<commit_message>
updated building energy use and baadtbvt
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/junshepard/library/containers/com.microsoft.excel/data/state-eps-data-repository/mn/trans/syvbt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C846A430-E998-A74B-A2F2-596EE06A205B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2A0B32-7816-974F-9D0F-640E04518890}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="2260" windowWidth="16360" windowHeight="14480" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11320" yWindow="2260" windowWidth="16360" windowHeight="14480" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="0" yWindow="680" windowWidth="19700" windowHeight="11580" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
@@ -6075,7 +6075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
@@ -6667,7 +6667,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
     <sheetView workbookViewId="1">

</xml_diff>